<commit_message>
More hurricane training results updates
</commit_message>
<xml_diff>
--- a/output/hurricane_inference.xlsx
+++ b/output/hurricane_inference.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgaligher/Desktop/OMSCS/DL_Fall25/final_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgaligher/Desktop/OMSCS/DL_Fall25/final_project/hurricane-cs7643/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEDCD32-A25A-7C43-B026-2B09FA58AEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7EFB8EA-7A27-A746-826A-6D3037CB76E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38420" yWindow="-4500" windowWidth="38400" windowHeight="21100" xr2:uid="{16077CE5-9C79-7842-920C-16E420B12397}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17380" xr2:uid="{16077CE5-9C79-7842-920C-16E420B12397}"/>
   </bookViews>
   <sheets>
     <sheet name="SAM-US Decoder" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Job ID</t>
   </si>
@@ -101,7 +101,25 @@
     <t>Final Score: 0.5471184209043152, Dice: 0.648257732207024, F1 (Harmonic Mean): 0.503773001774583, F1 (None): 0.7141705330747163, F1 (Minor): 0.5518264397153793, F1 (Major): 0.4271670418946744, F1 (Destroyed): 0.41898747927091556</t>
   </si>
   <si>
-    <t>Missing</t>
+    <t>Val Score: 0.5511806337268708, Dice: 0.6550187235030946, F1: 0.5066785952513463, F1_0: 0.7262694768791762, F1_1: 0.5533922882522604, F1_2: 0.4169374062598442, F1_3: 0.43249042623452677</t>
+  </si>
+  <si>
+    <t>Val Score: 0.5434696009142371, Dice: 0.6444403455583515, F1: 0.5001964246381881, F1_0: 0.7295705033550036, F1_1: 0.5657311055894948, F1_2: 0.40131980139256385, F1_3: 0.42251083235395687</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val Score: 0.5269342885172164, Dice: 0.5924285471543522, F1: 0.49886532052987237, F1_0: 0.7147454741081237, F1_1: 0.5357362183167285, F1_2: 0.4101912815415302, F1_3: 0.43203333773948216 </t>
+  </si>
+  <si>
+    <t>Val Score: 0.5248356290856423, Dice: 0.6038502582797844, F1: 0.4909722165738671, F1_0: 0.7210279094726519, F1_1: 0.5403606346097436, F1_2: 0.3931981933231123, F1_3: 0.4225923883650231</t>
+  </si>
+  <si>
+    <t>Val Score: 0.5144322468066552, Dice: 0.6356147390407136, F1: 0.4624968929920588, F1_0: 0.6801651195552217, F1_1: 0.5118687873752198, F1_2: 0.373868221363638, F1_3: 0.3921368319663758</t>
+  </si>
+  <si>
+    <t>Val Score: 0.5138224758304965, Dice: 0.6061634387730048, F1: 0.4742477774265643, F1_0: 0.7062714425012707, F1_1: 0.48687279436982683, F1_2: 0.38044838280366117, F1_3: 0.4280565530392445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val Score: 0.5501613593160817, Dice: 0.6525795916374272, F1: 0.5062678311783623, F1_0: 0.728876312405662, F1_1: 0.5447387677327333, F1_2: 0.4135657485837061, F1_3: 0.4395101811662328 </t>
   </si>
 </sst>
 </file>
@@ -109,7 +127,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -157,7 +175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -497,7 +515,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,189 +538,189 @@
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>3707212</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>3931841</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>3707260</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>3931832</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3887627</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>3707212</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>3791645</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>3797082</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
-        <v>3831725</v>
+        <v>3719676</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>3831723</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
+      <c r="A7" s="4">
+        <v>3791645</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>3698213</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
+      <c r="A8" s="4">
+        <v>3791773</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
-        <v>3698745</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>7</v>
+        <v>3944530</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
-        <v>3831775</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>9</v>
+        <v>3847917</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
-        <v>3719676</v>
+        <v>3707260</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>3791773</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>20</v>
+      <c r="A12" s="5">
+        <v>3698213</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
-        <v>3944530</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>3698745</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
-        <v>3944533</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="4">
+        <v>3797082</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
-        <v>12</v>
+      <c r="C14" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
-        <v>3931841</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>3831725</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
-        <v>3931832</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>13</v>
+        <v>3831723</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
-        <v>3887627</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>13</v>
+        <v>3831775</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
-        <v>3847917</v>
+        <v>3944533</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -720,6 +738,9 @@
       <c r="A20" s="5">
         <v>3797086</v>
       </c>
+      <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
@@ -728,34 +749,13 @@
       <c r="A21" s="5">
         <v>3797077</v>
       </c>
+      <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="C21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="5">
-        <v>3679047</v>
-      </c>
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
-        <v>3679008</v>
-      </c>
-      <c r="C23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
-        <v>3678995</v>
-      </c>
-      <c r="C24" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
     </row>
@@ -784,7 +784,12 @@
       <c r="A33" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{C63A9F49-F862-224A-A162-1B5CF63CAD5F}"/>
+  <autoFilter ref="A1:C1" xr:uid="{C63A9F49-F862-224A-A162-1B5CF63CAD5F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C21">
+      <sortCondition descending="1" ref="B1:B21"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Outline of changes in this commit: - Update of inference summary on latest dropout variant runs - Added references to additional files
</commit_message>
<xml_diff>
--- a/output/hurricane_inference.xlsx
+++ b/output/hurricane_inference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgaligher/Desktop/OMSCS/DL_Fall25/final_project/hurricane-cs7643/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7EFB8EA-7A27-A746-826A-6D3037CB76E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69936ABA-1156-2B47-9728-C5B650583FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17380" xr2:uid="{16077CE5-9C79-7842-920C-16E420B12397}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>Job ID</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t xml:space="preserve">Val Score: 0.5501613593160817, Dice: 0.6525795916374272, F1: 0.5062678311783623, F1_0: 0.728876312405662, F1_1: 0.5447387677327333, F1_2: 0.4135657485837061, F1_3: 0.4395101811662328 </t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>Final Score: 0.5321111841222543, Dice: 0.637605857036071, F1 (Harmonic Mean): 0.48689918144490446, F1 (None): 0.7068469068448531, F1 (Minor): 0.5547331976216221, F1 (Major): 0.4036499865486915, F1 (Destroyed): 0.3967506022091854</t>
+  </si>
+  <si>
+    <t>Final Score: 0.5234845775485619, Dice: 0.6475523757065577, F1 (Harmonic Mean): 0.47031266405227806, F1 (None): 0.6736148864535942, F1 (Minor): 0.5156041591187537, F1 (Major): 0.3893974149991026, F1 (Destroyed): 0.3979420441232515</t>
+  </si>
+  <si>
+    <t>Final Score: 0.17402245736147, Dice: 0.5800717467620095, F1 (Harmonic Mean): 1.3333326674042842e-06, F1 (None): 0.6674037680524672, F1 (Minor): 0.0, F1 (Major): 0.0, F1 (Destroyed): 0.0</t>
+  </si>
+  <si>
+    <t>Final Score: 0.5219593898711316, Dice: 0.6545977274446927, F1 (Harmonic Mean): 0.4651143880538911, F1 (None): 0.6735168254811738, F1 (Minor): 0.511743327025646, F1 (Major): 0.3898886279067426, F1 (Destroyed): 0.3851530017183201</t>
   </si>
 </sst>
 </file>
@@ -151,12 +166,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -171,13 +192,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,15 +547,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63A9F49-F862-224A-A162-1B5CF63CAD5F}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="208.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -536,113 +569,113 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
-        <v>3931841</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
+    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>3797082</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>3931832</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>3831725</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>3887627</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>3831723</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>3707212</v>
+        <v>3831775</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
-        <v>3719676</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>6</v>
+        <v>3944533</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
-        <v>3791645</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>3831775</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>3791773</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>3944530</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
+      <c r="A8" s="5">
+        <v>3797086</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>3797077</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>3847917</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="A10" s="6">
+        <v>3707212</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14">
         <v>3707260</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="12" t="s">
         <v>26</v>
       </c>
     </row>
@@ -669,95 +702,136 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>3797082</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>1</v>
+      <c r="A14" s="10">
+        <v>3791645</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
-        <v>3831725</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
+      <c r="A15" s="4">
+        <v>3791773</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
-        <v>3831723</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>3</v>
+      <c r="A16" s="6">
+        <v>3944530</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
-        <v>3831775</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>9</v>
+        <v>3847917</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>3944533</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
-        <v>3831775</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>3961657</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14">
+        <v>3961659</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
-        <v>3797086</v>
+        <v>3961660</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
-        <v>3797077</v>
+        <v>3961661</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>3719676</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>3931841</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>3931832</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
+      <c r="A25" s="5">
+        <v>3887627</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
@@ -785,8 +859,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{C63A9F49-F862-224A-A162-1B5CF63CAD5F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C21">
-      <sortCondition descending="1" ref="B1:B21"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C25">
+      <sortCondition ref="B1:B25"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>